<commit_message>
work on scheduler algo
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/nhs/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4AB0E6-A674-E44E-8B32-9280788C9339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDB8783-3D34-C141-9F1E-8A0D4005610B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17780" yWindow="-28300" windowWidth="30560" windowHeight="28300" activeTab="6" xr2:uid="{9F0F0AC9-5C7F-464B-8849-597E840CF182}"/>
+    <workbookView xWindow="-17780" yWindow="-28300" windowWidth="30560" windowHeight="28300" activeTab="3" xr2:uid="{9F0F0AC9-5C7F-464B-8849-597E840CF182}"/>
   </bookViews>
   <sheets>
     <sheet name="Table Design" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="200">
   <si>
     <t>2024-9-14</t>
   </si>
@@ -639,13 +639,16 @@
   </si>
   <si>
     <t>priority_id</t>
+  </si>
+  <si>
+    <t>month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -688,6 +691,12 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2384,18 +2393,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA4A713-A2B6-5240-AC23-FB68F49E0DD1}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>63</v>
       </c>
@@ -2406,10 +2416,13 @@
         <v>62</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2420,10 +2433,13 @@
         <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -2434,10 +2450,13 @@
         <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
@@ -2448,10 +2467,13 @@
         <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -2462,10 +2484,13 @@
         <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
@@ -2476,10 +2501,13 @@
         <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
@@ -2490,10 +2518,13 @@
         <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
@@ -2504,10 +2535,13 @@
         <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
@@ -2518,10 +2552,13 @@
         <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -2532,10 +2569,13 @@
         <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
@@ -2546,10 +2586,13 @@
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -2560,10 +2603,13 @@
         <v>27</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
@@ -2574,10 +2620,13 @@
         <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
@@ -2588,10 +2637,13 @@
         <v>60</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -2602,10 +2654,13 @@
         <v>59</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>61</v>
       </c>
@@ -2616,10 +2671,13 @@
         <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
@@ -2630,10 +2688,13 @@
         <v>57</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>59</v>
       </c>
@@ -2644,10 +2705,13 @@
         <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>58</v>
       </c>
@@ -2658,10 +2722,13 @@
         <v>55</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
@@ -2672,10 +2739,13 @@
         <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
@@ -2686,10 +2756,13 @@
         <v>53</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -2700,10 +2773,13 @@
         <v>52</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
@@ -2714,10 +2790,13 @@
         <v>51</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -2728,10 +2807,13 @@
         <v>50</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -2742,10 +2824,13 @@
         <v>49</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>51</v>
       </c>
@@ -2756,10 +2841,13 @@
         <v>48</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
@@ -2770,10 +2858,13 @@
         <v>47</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>49</v>
       </c>
@@ -2784,10 +2875,13 @@
         <v>46</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>48</v>
       </c>
@@ -2798,10 +2892,13 @@
         <v>44</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>47</v>
       </c>
@@ -2812,10 +2909,13 @@
         <v>4</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
@@ -2826,10 +2926,13 @@
         <v>45</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>44</v>
       </c>
@@ -2840,10 +2943,13 @@
         <v>43</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>42</v>
       </c>
@@ -2854,10 +2960,13 @@
         <v>41</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -2868,10 +2977,13 @@
         <v>39</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>20</v>
       </c>
@@ -2882,10 +2994,13 @@
         <v>38</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>17</v>
       </c>
@@ -2896,10 +3011,13 @@
         <v>37</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
@@ -2910,10 +3028,13 @@
         <v>36</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>11</v>
       </c>
@@ -2924,10 +3045,13 @@
         <v>35</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>8</v>
       </c>
@@ -2938,10 +3062,13 @@
         <v>34</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>5</v>
       </c>
@@ -2952,10 +3079,13 @@
         <v>33</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>32</v>
       </c>
@@ -2966,10 +3096,13 @@
         <v>31</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>30</v>
       </c>
@@ -2980,10 +3113,13 @@
         <v>29</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>28</v>
       </c>
@@ -2994,20 +3130,24 @@
         <v>27</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5603CB16-93C0-C14F-BA34-E42A0780428B}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3015,7 +3155,7 @@
     <col min="1" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -3026,19 +3166,22 @@
         <v>198</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -3049,19 +3192,22 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -3072,19 +3218,22 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3095,19 +3244,22 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3118,19 +3270,22 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3141,19 +3296,22 @@
         <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3164,15 +3322,18 @@
         <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3706,7 +3867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7006C3E6-2096-2047-B7FD-93A4752D6288}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>

</xml_diff>